<commit_message>
Did a good amount of work setting up our new protocol draft, and read part of 1 paper <3
</commit_message>
<xml_diff>
--- a/Medical Yearly Costs/CHAT prototype/Medical Cost Descriptions.xlsx
+++ b/Medical Yearly Costs/CHAT prototype/Medical Cost Descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Grad School\2022-2023\psych-phd\Medical Yearly Costs\CHAT prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06AD04F4-11A6-4C39-B1CE-1B97EC7ABE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCD4932-94E3-40F9-834A-2728FAB53A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2832" yWindow="3204" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Primary</t>
   </si>
@@ -45,21 +45,12 @@
     <t>Dental</t>
   </si>
   <si>
-    <t>Infertility</t>
-  </si>
-  <si>
-    <t>Last chance</t>
-  </si>
-  <si>
     <t>Long-Term</t>
   </si>
   <si>
     <t>Mental health and substance abuse</t>
   </si>
   <si>
-    <t>Other medical</t>
-  </si>
-  <si>
     <t>Specialty</t>
   </si>
   <si>
@@ -72,12 +63,6 @@
     <t>Basic</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -93,124 +78,124 @@
     <t>Pays for hospital bills - Note: except in an emergency, you need your insurance plan's approval before the hospital will admit you.</t>
   </si>
   <si>
-    <t>Pays for tests and special procedures for someone having trouble getting pregnant</t>
-  </si>
-  <si>
-    <t>Pays for special treatment in life-threatening situations like organ failure or extreme illness</t>
-  </si>
-  <si>
     <t>Pays for your care over a long period of time in a residential or nursing home</t>
   </si>
   <si>
     <t>Pays for counseling and therapy, treatment of mental illness, and alcohol and drug abuse</t>
   </si>
   <si>
-    <t>Pays for services and equipment like physical therapy, occupational therapy, ambulance service, wheel chair, hospital beds, and artificial limbs</t>
-  </si>
-  <si>
     <t>Pays for medicines your doctor prescribes</t>
   </si>
   <si>
     <t>Pays for regular care from your primary or “family” doctor and staff. Your primary doctor can refer you to other doctors, order special services, and coordinate your care</t>
   </si>
   <si>
-    <t>Pays for special problems your primary doctor and staff don't handle</t>
-  </si>
-  <si>
     <t>Pays for blood work, x-rays, or other tests you need</t>
   </si>
   <si>
     <t>Pays for eye exams, glasses, and contact lenses</t>
   </si>
   <si>
-    <t>1 peg: Covers “alternative” services including acupuncture (for pain), chiropractic (for back, neck or bone problems), and therapeutic massage.</t>
-  </si>
-  <si>
-    <t>2 pegs: You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. You get minimal dental care.</t>
-  </si>
-  <si>
-    <t>2 + 4 pegs: You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. You get complete dental care including repairs and crowns.</t>
-  </si>
-  <si>
-    <t>2 pegs: Your insurance pays in full for up to: 2 weekly visits from a nurse OR 2, 1/2 hr daily care from a nurse's aide.</t>
-  </si>
-  <si>
-    <t>2 + 1 pegs: Your insurance pays in full for up to: 4 weekly visits from a nurse OR 5 hr daily care from a nurse's aide.</t>
-  </si>
-  <si>
-    <t>10 pegs: You pay $50 per day for your first 5 days in the hospital. You have little choice about your hospital (i.e., it could be far from your home). There is pressure on your doctor to discharge you as soon as possible.</t>
-  </si>
-  <si>
-    <t>10 + 1 pegs: You pay nothing per day. You have a large selection of hospitals. There is probably one near your home. You have many special facilities to choose from. There is pressure on your doctor to discharge you as soon as possible.</t>
-  </si>
-  <si>
-    <t>10 + 1 + 3 pegs: You pay nothing per day. You have a large selection of hospitals. There's probably one near your home. You have many special facilities to choose from. Your doctor can keep you in the hospital as long as he/she wants.</t>
-  </si>
-  <si>
-    <t>1 peg: Infertility services are in the plan. However, expensive tests or procedures may require the insurance company's approval.</t>
-  </si>
-  <si>
-    <t>1 peg: Organ transplants are paid for by your plan.</t>
-  </si>
-  <si>
-    <t>1 + 1 pegs: Organ transplants are paid for by your plan. If you don't get better with current treatments, your insurance will pay for you to take part in research. You may get new treatments that are being tested.</t>
-  </si>
-  <si>
-    <t>4 pegs: Half your cost is paid for room and board in an average nursing home.</t>
-  </si>
-  <si>
-    <t>4 + 4 pegs: All your cost is paid for room and board in an average nursing home.</t>
-  </si>
-  <si>
-    <t>2 pegs: Your plan pays for up to 30 visits per year to a therapist. You pay $10 per visit. Your plan pays for up to 30 days per year in a hospital for mental illness or drug abuse. You pay $50 for each day in the hospital.</t>
-  </si>
-  <si>
-    <t>2 + 1 pegs: Your plan pays for an unlimited number of visits to a therapist or counselor. You pay nothing per visit. Your visits are free. Your plan pays for an unlimited number of days in a hospital for mental illness or drug abuse. You pay nothing for each day in the hospital.</t>
-  </si>
-  <si>
-    <t>2 pegs: Your health insurance company reviews your need first. Then it decides if it will pay for all, some, or none of the services or equipment requested.</t>
-  </si>
-  <si>
-    <t>2 + 1 pegs: There is no review process. Your health plan pays in full for all services and equipment</t>
-  </si>
-  <si>
-    <t>3 pegs: Your health plan only pays for medicines on its approved list (formulary). If your are prescribed a medicine not on this list, either your doctor has to change it or you pay for it. Your pharmacist must give you a generic medicine if he/she has it. You pay $15 per prescription.</t>
-  </si>
-  <si>
-    <t>3 + 3 pegs: Your health plan only pays for medicines on its formulary. If you are prescribed a medicine not on this list, either your doctor has to change it or you pay for it. Your pharmacist may use either generic or brand name medicines for your prescriptions. You pay $5 for generic drugs or $10 for brand name drugs.</t>
-  </si>
-  <si>
-    <t>3 + 3 + 2 pegs: Your health plan is not limited by the formulary. Your pharmacist may use either generic or brand name medicines for your prescriptions. You pay $5 per prescription.</t>
-  </si>
-  <si>
-    <t>4 pegs: You pay $10 per visit. You wait about 4 weeks for a routine appointment and about 48 hours for an urgent problem. You pay $25 per emergency room visit. There are few doctors from which to choose. It may be difficult to see the doctor you have now, or to pick a female or a minority doctor, or a doctor who speaks your language. You may sometimes see a nurse or physician's assistant instead of a doctor.</t>
-  </si>
-  <si>
-    <t>4 + 1 pegs: You pay $10 per visit. You wait about 2 weeks for a routine appointment. You wait about 24 hours for an urgent problem. You pay nothing for emergency room visits. You have more doctors to choose from. You have a better chance of seeing the doctor you have now, or to pick a female or a minority doctor, or a doctor who speaks your language. You'll usually see a doctor rather than a nurse or physician's assistant.</t>
-  </si>
-  <si>
-    <t>4 + 1 + 1 pegs: Your plan has all the medium levels plus wellness and prevention benefits such as stop smoking programs, diet programs, automatic cancer screening, and stress management.</t>
-  </si>
-  <si>
-    <t>9 pegs: You need your primary doctor's referral to see a specialist in your plan. You wait about 45 days for an appointment. There are few specialists available. You have little choice of which doctor you see. You pay $10 a visit. If you visit a specialist outside of your plan or go without a referral, you pay for it.</t>
-  </si>
-  <si>
-    <t>9 + 2 pegs: You may see a specialist in your plan without a referral from your primary doctor. You wait about 25 days for an appointment. There are more specialists available. You have more choice of which doctor you see. You pay $10 a visit. If you visit a specialist outside of your plan or go without a referral, you pay half.</t>
-  </si>
-  <si>
-    <t>9 + 2 + 5 pegs: You may see a specialist without a referral from your primary doctor. You wait only a few days for an appointment. There are many specialties available. You may go to almost any specialist in your area. You pay $10 per visit.</t>
-  </si>
-  <si>
-    <t>3 pegs: Your doctor needs to get expensive tests approved before ordering them. You might need the test done at a lab far away from your doctor's office.</t>
-  </si>
-  <si>
-    <t>3 + 1 pegs: Your doctor can order any tests for you without getting approval. You can have the tests done at or near your doctor's office.</t>
-  </si>
-  <si>
-    <t>1 peg: You get an eye exam every 2 years.</t>
-  </si>
-  <si>
-    <t>1 + 1 peg: You get an eye exam every 2 years. You pay $5 per visit. You receive $75 for lenses and frames if needed every 2 years.</t>
+    <t>Medical Equipment</t>
+  </si>
+  <si>
+    <t>Pays for equipment like wheel chairs, hearing aids, and artificial limbs</t>
+  </si>
+  <si>
+    <t>Professional services including chiropractors, physical therapists, podiatrists and others</t>
+  </si>
+  <si>
+    <t>10 points: You pay $50 per day for your first 5 days in the hospital. You have little choice about your hospital (i.e., it could be far from your home). There is pressure on your doctor to discharge you as soon as possible.</t>
+  </si>
+  <si>
+    <t>4 points: You pay $10 per visit. You wait about 4 weeks for a routine appointment and about 48 hours for an urgent problem. You pay $25 per emergency room visit. There are few doctors from which to choose. It may be difficult to see the doctor you have now, or to pick a female or a minority doctor, or a doctor who speaks your language. You may sometimes see a nurse or physician's assistant instead of a doctor.</t>
+  </si>
+  <si>
+    <t>3 points: Your health plan only pays for medicines on its approved list (formulary). If your are prescribed a medicine not on this list, either your doctor has to change it or you pay for it. Your pharmacist must give you a generic medicine if he/she has it. You pay $15 per prescription.</t>
+  </si>
+  <si>
+    <t>4 points: Half your cost is paid for room and board in an average nursing home.</t>
+  </si>
+  <si>
+    <t>4 + 4 points: All your cost is paid for room and board in an average nursing home.</t>
+  </si>
+  <si>
+    <t>2 points: Your plan pays for up to 30 visits per year to a therapist. You pay $10 per visit. Your plan pays for up to 30 days per year in a hospital for mental illness or drug abuse. You pay $50 for each day in the hospital.</t>
+  </si>
+  <si>
+    <t>2 + 1 points: Your plan pays for an unlimited number of visits to a therapist or counselor. You pay nothing per visit. Your visits are free. Your plan pays for an unlimited number of days in a hospital for mental illness or drug abuse. You pay nothing for each day in the hospital.</t>
+  </si>
+  <si>
+    <t>2 points: You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. You get minimal dental care.</t>
+  </si>
+  <si>
+    <t>2 + 4 points: You get regular cleanings and x-rays every 6 months. You have cavities filled and bad teeth extracted. You get complete dental care including repairs and crowns.</t>
+  </si>
+  <si>
+    <t>2 points: Your insurance pays in full for up to: 2 weekly visits from a nurse OR 2, 1/2 hr daily care from a nurse's aide.</t>
+  </si>
+  <si>
+    <t>2 + 1 points: Your insurance pays in full for up to: 4 weekly visits from a nurse OR 5 hr daily care from a nurse's aide.</t>
+  </si>
+  <si>
+    <t>1 point: Your health insurance company reviews your need first. Then it decides if it will pay for all, some, or none of the equipment requested.</t>
+  </si>
+  <si>
+    <t>1+ 1 points: There is no review process. Your health plan pays in full for all and equipment</t>
+  </si>
+  <si>
+    <t>1 point: You get an eye exam every 2 years.</t>
+  </si>
+  <si>
+    <t>1 + 1 point: You get an eye exam every 2 years. You pay $5 per visit. You receive $75 for lenses and frames if needed every 2 years.</t>
+  </si>
+  <si>
+    <t>1 point: Covers “alternative” services including acupuncture (for pain), chiropractic (for back, neck or bone problems), and therapeutic massage.</t>
+  </si>
+  <si>
+    <t>3 points: Your doctor needs to get expensive tests approved before ordering them. You might need the test done at a lab far away from your doctor's office.</t>
+  </si>
+  <si>
+    <t>3 + 1 points: Your doctor can order any tests for you without getting approval. You can have the tests done at or near your doctor's office.</t>
+  </si>
+  <si>
+    <t>7 points: You need your primary doctor's referral to see a specialist in your plan. You wait about 45 days for an appointment. There are few specialists available. You have little choice of which doctor you see. You pay $10 a visit. If you visit a specialist outside of your plan or go without a referral, you pay for it.</t>
+  </si>
+  <si>
+    <t>7 + 7 points: You may see a specialist without a referral from your primary doctor. You wait only a few days for an appointment. There are many specialties available. You may go to almost any specialist in your area. You pay $10 per visit.</t>
+  </si>
+  <si>
+    <t>10 + 4 points: You pay nothing per day. You have a large selection of hospitals. There's probably one near your home. You have many special facilities to choose from. Your doctor can keep you in the hospital as long as he/she wants.</t>
+  </si>
+  <si>
+    <t>4 + 2 points: You pay $10 per visit. You wait about 2 weeks for a routine appointment. You wait about 24 hours for an urgent problem. You pay nothing for emergency room visits. You have more doctors to choose from. You have a better chance of seeing the doctor you have now, or to pick a female or a minority doctor, or a doctor who speaks your language. You'll usually see a doctor rather than a nurse or physician's assistant. There are also wellness and prevention benefits such as stop smoking programs, diet programs, automatic cancer screening, and stress management.</t>
+  </si>
+  <si>
+    <t>3 + 5 points: Your health plan is not limited by the formulary. Your pharmacist may use either generic or brand name medicines for your prescriptions. You pay $5 per prescription.</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>originally 47/72</t>
+  </si>
+  <si>
+    <t>70 total.. Try 45/46?</t>
+  </si>
+  <si>
+    <t>Total personal health care (total that should be spent outside of investment/administrative fees) in mil = 3357832</t>
+  </si>
+  <si>
+    <t>Yearly spent by private health insurance = 1,000,234</t>
+  </si>
+  <si>
+    <t>Yearly spent by Govt health insurance = 1,490,818</t>
+  </si>
+  <si>
+    <t>Group Market = 54.4%, individual market = 10.5%</t>
+  </si>
+  <si>
+    <t>Medicare = 18.4%, Medicaid/CHIP = 17.8%, VA/TRICARE = 2.8+0.9%</t>
   </si>
 </sst>
 </file>
@@ -295,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -314,6 +299,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +650,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -667,240 +661,213 @@
     <col min="1" max="1" width="30.5546875" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="3" width="34.88671875" customWidth="1"/>
-    <col min="4" max="4" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="122.4" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="102.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="52.8" x14ac:dyDescent="0.5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="61.2" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="52.8" x14ac:dyDescent="0.5">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="52.8" x14ac:dyDescent="0.5">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="79.2" x14ac:dyDescent="0.5">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="52.8" x14ac:dyDescent="0.5">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="52.8" x14ac:dyDescent="0.5">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="52.8" x14ac:dyDescent="0.5">
-      <c r="A8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="61.2" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="52.8" x14ac:dyDescent="0.5">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="92.4" x14ac:dyDescent="0.5">
+    </row>
+    <row r="10" spans="1:7" ht="51.6" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="102.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="92.4" x14ac:dyDescent="0.5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="71.400000000000006" x14ac:dyDescent="0.5">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="4"/>
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created our java exercise for our new protocol, MOSTLY finished our add-in sheet w/ descriptions. Still need a calibrated costs burden (out of pocket and insurance costs).
</commit_message>
<xml_diff>
--- a/Medical Yearly Costs/CHAT prototype/Medical Cost Descriptions.xlsx
+++ b/Medical Yearly Costs/CHAT prototype/Medical Cost Descriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Grad School\2022-2023\psych-phd\Medical Yearly Costs\CHAT prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCD4932-94E3-40F9-834A-2728FAB53A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8AD02C-37A6-48CD-9FAA-F05313ECAF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="3204" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16728" yWindow="5388" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,9 +150,6 @@
     <t>1 + 1 point: You get an eye exam every 2 years. You pay $5 per visit. You receive $75 for lenses and frames if needed every 2 years.</t>
   </si>
   <si>
-    <t>1 point: Covers “alternative” services including acupuncture (for pain), chiropractic (for back, neck or bone problems), and therapeutic massage.</t>
-  </si>
-  <si>
     <t>3 points: Your doctor needs to get expensive tests approved before ordering them. You might need the test done at a lab far away from your doctor's office.</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Medicare = 18.4%, Medicaid/CHIP = 17.8%, VA/TRICARE = 2.8+0.9%</t>
+  </si>
+  <si>
+    <t>1 point: Covers “alternative” services including acupuncture (for pain), spiritual healing or Reiki, and therapeutic massage.</t>
   </si>
 </sst>
 </file>
@@ -652,8 +652,8 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -678,13 +678,13 @@
         <v>12</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
         <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="100.8" x14ac:dyDescent="0.5">
@@ -698,10 +698,10 @@
         <v>27</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2" s="7"/>
     </row>
@@ -716,13 +716,13 @@
         <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="102.6" customHeight="1" x14ac:dyDescent="0.5">
@@ -736,13 +736,13 @@
         <v>29</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="52.8" x14ac:dyDescent="0.5">
@@ -809,10 +809,10 @@
         <v>26</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="51.6" x14ac:dyDescent="0.5">
@@ -851,7 +851,7 @@
         <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -863,10 +863,10 @@
         <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>